<commit_message>
before removing add. progress
</commit_message>
<xml_diff>
--- a/outputs/filtered_sites.xlsx
+++ b/outputs/filtered_sites.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>village</t>
   </si>
@@ -25,43 +25,19 @@
     <t>habitation</t>
   </si>
   <si>
-    <t>KAKCHING KHUNOU</t>
-  </si>
-  <si>
-    <t>ATHOKPAM</t>
-  </si>
-  <si>
-    <t>SIKHONG SEKMAI</t>
-  </si>
-  <si>
-    <t>YAIRIPOK</t>
-  </si>
-  <si>
-    <t>SUGNU</t>
-  </si>
-  <si>
-    <t>801483</t>
-  </si>
-  <si>
-    <t>801479</t>
-  </si>
-  <si>
-    <t>801480</t>
-  </si>
-  <si>
-    <t>801481</t>
-  </si>
-  <si>
-    <t>801482</t>
-  </si>
-  <si>
-    <t>NAN</t>
-  </si>
-  <si>
-    <t>MATHAK LEIKAI</t>
-  </si>
-  <si>
-    <t>KAKCHING KHUMAN</t>
+    <t>TENGKHAL KHUNOU</t>
+  </si>
+  <si>
+    <t>269882</t>
+  </si>
+  <si>
+    <t>TENGKHAL KHUNOUA</t>
+  </si>
+  <si>
+    <t>TENKHAL KHUNOU A</t>
+  </si>
+  <si>
+    <t>TENKHAL KHUNOU</t>
   </si>
 </sst>
 </file>
@@ -419,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,10 +420,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -455,69 +431,41 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
         <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>